<commit_message>
Criando script para somer
</commit_message>
<xml_diff>
--- a/aula333/workbook.xlsx
+++ b/aula333/workbook.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Empresa1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -424,12 +424,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Nome</t>
+          <t>Exame</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Idade</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>João</t>
+          <t>teste1</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -454,11 +454,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Maria</t>
+          <t>teste2</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C3" t="n">
         <v>9.699999999999999</v>
@@ -467,7 +467,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Luiz</t>
+          <t>teste3</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -480,7 +480,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Alberto</t>
+          <t>teste4</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>